<commit_message>
Jean's suggestion on Human in the loop for consideration
</commit_message>
<xml_diff>
--- a/SelectedParticipants.xlsx
+++ b/SelectedParticipants.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eriak\Documents\NTU\Trimester 3\AN6817 RPA for Analytics\Group Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enaij\OneDrive - Nanyang Technological University\Documents\MSBA Materials\AN6817 - RPA\Projects\GroupAssg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B510693-D3DA-4F5C-81B6-19838072A15D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0BC0E84-9D92-4315-BE0B-D4822499AF06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="0" windowWidth="14400" windowHeight="9320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="30960" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="50">
   <si>
     <t>Timestamp</t>
   </si>
@@ -164,6 +164,12 @@
   </si>
   <si>
     <t>ERI001@e.ntu.edu.sg</t>
+  </si>
+  <si>
+    <t>Dr. John Williams</t>
+  </si>
+  <si>
+    <t>Candice Washington</t>
   </si>
 </sst>
 </file>
@@ -513,15 +519,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.21875" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" customWidth="1"/>
+    <col min="5" max="5" width="53.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -541,7 +553,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>45417.834606481498</v>
       </c>
@@ -561,7 +573,7 @@
         <v>14583376</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>45418.152708333299</v>
       </c>
@@ -581,7 +593,7 @@
         <v>15480124</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>45416.657222222202</v>
       </c>
@@ -601,7 +613,7 @@
         <v>19760685</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>45418.502638888902</v>
       </c>
@@ -621,7 +633,7 @@
         <v>22789443</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>45419.741041666697</v>
       </c>
@@ -641,7 +653,7 @@
         <v>24219363</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>45418.5249652778</v>
       </c>
@@ -661,7 +673,7 @@
         <v>24770454</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>45416.004884259302</v>
       </c>
@@ -681,7 +693,7 @@
         <v>26663693</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>45418.074513888903</v>
       </c>
@@ -701,7 +713,7 @@
         <v>36373341</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>45417.565219907403</v>
       </c>
@@ -721,7 +733,7 @@
         <v>37105247</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>45418.524780092601</v>
       </c>
@@ -741,7 +753,7 @@
         <v>38559467</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>45419.872337963003</v>
       </c>
@@ -761,7 +773,7 @@
         <v>39467735</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>45419.290740740696</v>
       </c>
@@ -781,7 +793,7 @@
         <v>41370596</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>45418.899872685201</v>
       </c>
@@ -801,7 +813,7 @@
         <v>42487189</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>45417.960914351897</v>
       </c>
@@ -821,7 +833,7 @@
         <v>42910376</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>45417.620914351799</v>
       </c>
@@ -841,7 +853,7 @@
         <v>45345003</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>45419.701435185198</v>
       </c>
@@ -861,7 +873,7 @@
         <v>58574868</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>45419.654490740701</v>
       </c>
@@ -881,7 +893,7 @@
         <v>62193437</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>45416.639594907399</v>
       </c>
@@ -901,7 +913,7 @@
         <v>62283126</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>45419.332673611098</v>
       </c>
@@ -921,7 +933,7 @@
         <v>62798342</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>45416.013541666704</v>
       </c>
@@ -941,7 +953,7 @@
         <v>67424150</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>45416.033449074101</v>
       </c>
@@ -961,7 +973,7 @@
         <v>67431110</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>45418.4749884259</v>
       </c>
@@ -981,7 +993,7 @@
         <v>69526335</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>45416.582650463002</v>
       </c>
@@ -1001,7 +1013,7 @@
         <v>71034050</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>45419.117881944403</v>
       </c>
@@ -1021,7 +1033,7 @@
         <v>72696126</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>45416.431099537003</v>
       </c>
@@ -1041,7 +1053,7 @@
         <v>88062606</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>45419.1336226852</v>
       </c>
@@ -1061,7 +1073,7 @@
         <v>89431443</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>45416.009814814803</v>
       </c>
@@ -1081,7 +1093,7 @@
         <v>91762639</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>45416.406226851897</v>
       </c>
@@ -1101,7 +1113,7 @@
         <v>92312909</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>45418.010671296302</v>
       </c>
@@ -1121,7 +1133,7 @@
         <v>93038340</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>45416.752858796302</v>
       </c>
@@ -1141,7 +1153,7 @@
         <v>93268593</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>45418.2479282407</v>
       </c>
@@ -1161,7 +1173,7 @@
         <v>94192223</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>45418.004039351901</v>
       </c>
@@ -1181,7 +1193,7 @@
         <v>95425054</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>45417.710347222201</v>
       </c>
@@ -1201,7 +1213,7 @@
         <v>98427834</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>45419.996168981503</v>
       </c>
@@ -1219,6 +1231,46 @@
       </c>
       <c r="F35">
         <v>99338799</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>45418.502638888902</v>
+      </c>
+      <c r="B36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" t="s">
+        <v>20</v>
+      </c>
+      <c r="F36">
+        <v>30338111</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>45419.1320949074</v>
+      </c>
+      <c r="B37" t="s">
+        <v>49</v>
+      </c>
+      <c r="C37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" t="s">
+        <v>16</v>
+      </c>
+      <c r="E37" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37">
+        <v>87857672</v>
       </c>
     </row>
   </sheetData>

</xml_diff>